<commit_message>
added a comment in xlsx file
</commit_message>
<xml_diff>
--- a/Task_9/Sales_Data.xlsx
+++ b/Task_9/Sales_Data.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>Laptop</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Bonus Rate</t>
+  </si>
+  <si>
+    <t>How to fix the error in cell J2</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +254,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,40 +425,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -494,13 +478,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -516,30 +493,44 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -577,11 +568,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="M3:N8" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="M3:N8" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="M3:N8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Profit" dataDxfId="2"/>
-    <tableColumn id="2" name="Bonus Rate" dataDxfId="1"/>
+    <tableColumn id="1" name="Profit" dataDxfId="1"/>
+    <tableColumn id="2" name="Bonus Rate" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -853,7 +844,7 @@
   <dimension ref="A1:V5316"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45729</v>
       </c>
@@ -1329,6 +1320,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="M12" s="22" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1640,7 +1634,7 @@
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="5311" spans="21:22" x14ac:dyDescent="0.25">
+    <row r="5311" spans="21:22" ht="30" x14ac:dyDescent="0.25">
       <c r="U5311" s="5" t="s">
         <v>31</v>
       </c>
@@ -1695,12 +1689,12 @@
     <sortCondition ref="C2:C38"/>
   </sortState>
   <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>499</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H21">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>